<commit_message>
Schedule 姚波 for xiaoyusan.cps.product.detail.page
</commit_message>
<xml_diff>
--- a/项目管理工具文档.xlsx
+++ b/项目管理工具文档.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28660" windowHeight="13320"/>
+    <workbookView windowWidth="28695" windowHeight="13185"/>
   </bookViews>
   <sheets>
     <sheet name="每周排期" sheetId="1" r:id="rId1"/>
     <sheet name="项目节点管理" sheetId="5" r:id="rId2"/>
     <sheet name="唐僧保3.3" sheetId="2" r:id="rId3"/>
     <sheet name="深爱保2.0" sheetId="3" r:id="rId4"/>
-    <sheet name="开发团队" sheetId="4" r:id="rId5"/>
+    <sheet name="深爱保2.1" sheetId="6" r:id="rId5"/>
+    <sheet name="开发团队" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">唐僧保3.3!$E$4</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124">
   <si>
     <t>排期日期</t>
   </si>
@@ -314,6 +315,12 @@
     <t>(8) 一保到位对接</t>
   </si>
   <si>
+    <t>(9) 小雨伞五款cps合作产品的详情页面 - A端</t>
+  </si>
+  <si>
+    <t>周二至周四</t>
+  </si>
+  <si>
     <t>项目节点管理</t>
   </si>
   <si>
@@ -429,6 +436,12 @@
   </si>
   <si>
     <t>移动端官网以及资源服务器搬迁 - 解决音频流量过大</t>
+  </si>
+  <si>
+    <t>此版本为深爱保微信网页版</t>
+  </si>
+  <si>
+    <t>小雨伞五款cps合作产品的详情页面 - A端</t>
   </si>
   <si>
     <t>3+2+1模式</t>
@@ -451,9 +464,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
@@ -516,6 +529,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -530,6 +550,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -538,7 +566,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -553,7 +581,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -561,14 +589,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -583,16 +619,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -601,6 +630,20 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -616,37 +659,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -687,7 +700,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -699,7 +814,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -711,90 +850,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -807,7 +862,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -819,49 +874,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -995,32 +1008,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1030,6 +1019,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1049,6 +1047,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1064,13 +1073,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1094,148 +1107,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1279,6 +1292,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1336,9 +1355,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1353,9 +1369,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1435,7 +1448,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="4D4D4D"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1715,28 +1728,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:XFD69"/>
+  <dimension ref="A1:XFD71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="K64" sqref="K64"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="69.8" customWidth="1"/>
     <col min="2" max="2" width="10.6" style="6" customWidth="1"/>
     <col min="3" max="3" width="13" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.88" style="6" customWidth="1"/>
+    <col min="4" max="4" width="12.8833333333333" style="6" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="12.88" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.8833333333333" style="6" customWidth="1"/>
     <col min="7" max="7" width="18.25" customWidth="1"/>
     <col min="9" max="9" width="8.4" customWidth="1"/>
     <col min="10" max="10" width="6.2" customWidth="1"/>
     <col min="11" max="11" width="8.4" customWidth="1"/>
     <col min="12" max="14" width="6.2" customWidth="1"/>
-    <col min="18" max="18" width="17.13" customWidth="1"/>
+    <col min="18" max="18" width="17.1333333333333" customWidth="1"/>
     <col min="19" max="19" width="7" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1784,7 +1797,7 @@
       <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="F6"/>
@@ -1800,27 +1813,27 @@
       <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="13"/>
+      <c r="D7" s="15"/>
       <c r="F7"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="6:19">
+    <row r="8" ht="15.75" spans="6:19">
       <c r="F8"/>
       <c r="G8" s="6"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="25" t="s">
+      <c r="I8" s="26"/>
+      <c r="J8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="25" t="s">
+      <c r="L8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="25" t="s">
+      <c r="M8" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="33" t="s">
+      <c r="N8" s="34" t="s">
         <v>18</v>
       </c>
       <c r="P8" s="1" t="s">
@@ -1846,29 +1859,29 @@
       <c r="C9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="6"/>
       <c r="I9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="M9" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="N9" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="P9" s="35" t="s">
+      <c r="J9" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" s="36" t="s">
         <v>24</v>
       </c>
       <c r="Q9" s="8" t="s">
@@ -1891,17 +1904,17 @@
       <c r="C10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="6"/>
       <c r="I10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J10" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="26" t="s">
+      <c r="J10" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="28" t="s">
         <v>12</v>
       </c>
       <c r="L10" s="6"/>
@@ -1913,19 +1926,19 @@
       <c r="I11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="L11" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="M11" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="N11" s="34" t="s">
+      <c r="J11" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" s="35" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1939,20 +1952,20 @@
       <c r="C12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="6"/>
       <c r="I12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="L12" s="26" t="s">
+      <c r="J12" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="28" t="s">
         <v>12</v>
       </c>
       <c r="M12" s="6"/>
@@ -1963,19 +1976,19 @@
       <c r="I13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="L13" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="M13" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="N13" s="36" t="s">
+      <c r="J13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13" s="37" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1989,7 +2002,7 @@
       <c r="C14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G14" s="6"/>
@@ -2000,7 +2013,7 @@
     </row>
     <row r="15" spans="7:10">
       <c r="G15" s="6"/>
-      <c r="J15" s="26"/>
+      <c r="J15" s="28"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
@@ -2036,7 +2049,7 @@
       <c r="C18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G18" s="6"/>
@@ -2054,7 +2067,7 @@
       <c r="C20" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="6"/>
@@ -2072,7 +2085,7 @@
       <c r="C22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="6"/>
@@ -2087,13 +2100,13 @@
       <c r="C23" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="6"/>
     </row>
     <row r="24" spans="4:7">
-      <c r="D24" s="13"/>
+      <c r="D24" s="15"/>
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7">
@@ -2106,7 +2119,7 @@
       <c r="C25" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="13"/>
+      <c r="D25" s="15"/>
       <c r="G25" s="6"/>
     </row>
     <row r="26" spans="7:7">
@@ -2122,7 +2135,7 @@
       <c r="C27" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="21" t="s">
         <v>20</v>
       </c>
       <c r="G27" s="6" t="s">
@@ -2139,7 +2152,7 @@
       <c r="C28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="21" t="s">
         <v>20</v>
       </c>
       <c r="G28" s="6" t="s">
@@ -2159,7 +2172,7 @@
       <c r="C30" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="22" t="s">
         <v>21</v>
       </c>
       <c r="G30" s="6"/>
@@ -2177,7 +2190,7 @@
       <c r="C32" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G32" s="6"/>
@@ -2195,10 +2208,10 @@
       <c r="C34" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="23" t="s">
+      <c r="D34" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="25" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2206,7 +2219,7 @@
       <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="23" t="s">
         <v>51</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -2215,7 +2228,7 @@
       <c r="C36" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="15" t="s">
         <v>12</v>
       </c>
       <c r="F36" s="6" t="s">
@@ -2233,7 +2246,7 @@
       <c r="C38" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G38" t="s">
@@ -2241,7 +2254,7 @@
       </c>
     </row>
     <row r="39" spans="4:4">
-      <c r="D39" s="13"/>
+      <c r="D39" s="15"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
@@ -2253,7 +2266,7 @@
       <c r="C40" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="22" t="s">
         <v>21</v>
       </c>
       <c r="G40" t="s">
@@ -2270,7 +2283,7 @@
       <c r="C42" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="22" t="s">
         <v>21</v>
       </c>
       <c r="G42" t="s">
@@ -2287,12 +2300,12 @@
       <c r="C44" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B46" s="6" t="s">
@@ -2301,41 +2314,41 @@
       <c r="C46" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D46" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="9:14">
-      <c r="I49" s="28" t="s">
+      <c r="D46" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" ht="15.75" spans="9:14">
+      <c r="I49" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="J49" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K49" s="30" t="s">
+      <c r="J49" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="K49" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="L49" s="31" t="s">
+      <c r="L49" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="M49" s="30"/>
-      <c r="N49" s="37"/>
+      <c r="M49" s="32"/>
+      <c r="N49" s="38"/>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I50" s="5"/>
-      <c r="J50" s="22" t="s">
+      <c r="J50" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="K50" s="22" t="s">
+      <c r="K50" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="L50" s="22" t="s">
+      <c r="L50" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="M50" s="22" t="s">
+      <c r="M50" s="24" t="s">
         <v>17</v>
       </c>
       <c r="N50" s="11" t="s">
@@ -2349,24 +2362,24 @@
       <c r="I51" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J51" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="K51" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="L51" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="M51" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="N51" s="34" t="s">
+      <c r="J51" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K51" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L51" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="M51" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N51" s="35" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B52" s="6" t="s">
@@ -2378,19 +2391,19 @@
       <c r="I52" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J52" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="K52" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="L52" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="M52" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="N52" s="38" t="s">
+      <c r="J52" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L52" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="M52" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N52" s="35" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2398,19 +2411,19 @@
       <c r="I53" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J53" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="K53" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="L53" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="M53" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="N53" s="34" t="s">
+      <c r="J53" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K53" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L53" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="M53" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N53" s="35" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2427,37 +2440,37 @@
       <c r="I54" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J54" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="K54" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="L54" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="M54" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="N54" s="34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="9:14">
+      <c r="J54" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K54" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L54" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="M54" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N54" s="35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" ht="15.75" spans="9:14">
       <c r="I55" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J55" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="K55" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="L55" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="M55" s="32" t="s">
-        <v>21</v>
+      <c r="J55" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K55" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="L55" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="M55" s="29" t="s">
+        <v>12</v>
       </c>
       <c r="N55" s="39" t="s">
         <v>21</v>
@@ -2478,7 +2491,7 @@
       <c r="A57" t="s">
         <v>66</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="24" t="s">
         <v>10</v>
       </c>
       <c r="C57" s="6" t="s">
@@ -2519,7 +2532,7 @@
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="21" t="s">
+      <c r="A65" s="23" t="s">
         <v>70</v>
       </c>
       <c r="B65" s="6" t="s">
@@ -2569,6 +2582,17 @@
       </c>
       <c r="C69" s="6" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2596,7 +2620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -2604,7 +2628,7 @@
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" outlineLevelRow="4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="10.6" style="6" customWidth="1"/>
@@ -2616,101 +2640,101 @@
   </cols>
   <sheetData>
     <row r="1" ht="37" customHeight="1" spans="1:8">
-      <c r="A1" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="A1" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="17">
+        <v>86</v>
+      </c>
+      <c r="B3" s="19">
         <v>43313</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H3" s="18">
+        <v>90</v>
+      </c>
+      <c r="H3" s="20">
         <v>43317</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="17">
+        <v>91</v>
+      </c>
+      <c r="B4" s="19">
         <v>43313</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="18">
+      <c r="H4" s="20">
         <v>43317</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="17">
+        <v>93</v>
+      </c>
+      <c r="B5" s="19">
         <v>43306</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2723,15 +2747,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9" style="4"/>
     <col min="2" max="2" width="64.4" customWidth="1"/>
@@ -2742,22 +2766,22 @@
     <col min="7" max="7" width="22.75" customWidth="1"/>
     <col min="9" max="9" width="19.4" customWidth="1"/>
     <col min="11" max="11" width="22.75" customWidth="1"/>
-    <col min="12" max="12" width="16.13" customWidth="1"/>
-    <col min="15" max="15" width="19.13" style="6" customWidth="1"/>
+    <col min="12" max="12" width="16.1333333333333" customWidth="1"/>
+    <col min="15" max="15" width="19.1333333333333" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>7</v>
@@ -2771,16 +2795,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2788,23 +2812,23 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
+        <v>105</v>
+      </c>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
     </row>
     <row r="5" spans="9:9">
       <c r="I5" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2812,43 +2836,43 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="9:9">
       <c r="I7" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>108</v>
+      <c r="B8" s="16" t="s">
+        <v>110</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4">
         <v>5</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>111</v>
+      <c r="B10" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>27</v>
@@ -2862,10 +2886,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="5:5">
@@ -2876,10 +2900,10 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="5:5">
@@ -2893,10 +2917,10 @@
         <v>49</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="5:5">
@@ -2907,10 +2931,10 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2926,16 +2950,36 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
@@ -2943,7 +2987,65 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="37.875" customWidth="1"/>
+    <col min="3" max="3" width="12.875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="12.875" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="14">
+        <v>43318</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="B2:F7"/>
   <sheetViews>
@@ -2951,20 +3053,20 @@
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" outlineLevelRow="6" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="10.88" customWidth="1"/>
+    <col min="1" max="1" width="10.8833333333333" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="10.88" customWidth="1"/>
+    <col min="3" max="3" width="10.8833333333333" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="10.88" customWidth="1"/>
+    <col min="5" max="5" width="10.8833333333333" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="9" max="9" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2980,15 +3082,15 @@
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="10" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="2:6">
@@ -3001,7 +3103,7 @@
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="11" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="2:6">

</xml_diff>